<commit_message>
Refactor your static page into your Fortune-of-the-Day website (JAVA 11) which reads/updates a list of fortunes in the AWS DynamoDB table. (Hint: EC2 Instance Role) Add CloudFormation File
</commit_message>
<xml_diff>
--- a/external-data/2_advanced_fortune_app/2_advanced_fortune_app.xlsx
+++ b/external-data/2_advanced_fortune_app/2_advanced_fortune_app.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NamNVH\Desktop\AWS\aws-challenge\external-data\2_advanced_fortune_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7020A0-4F5A-4A1A-ABAD-BF7B6C67DDF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6065CC0E-F7AF-468C-815A-E1C186FE9F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+  <si>
+    <t>Run as -&gt; Maven build … -&gt; Goals: package</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qDTUYkaXAEc</t>
+  </si>
+  <si>
+    <t>https://intellipaat.com/community/43019/how-to-copy-files-from-local-machine-to-my-aws-instance</t>
+  </si>
+  <si>
+    <t>https://github.com/hn310/aws-challenge/tree/master/external-data/2_advanced_fortune_app</t>
+  </si>
+  <si>
+    <t>A. Manual</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>①．Build jar for "fortune of the day" spring project</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>・Option 1: Use the code in aws folder to customize on your own</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>・Option 2: Use aws-0.0.1-SNAPSHOT.jar if you want to deploy straight away without rebuilding the project</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>How to build jar in details</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>②．Create EC2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2.1. Create EC2 instance with inbound allow port 8080</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2.2. Install java 11 on EC2 to run jar file</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2.3. Attach DynamoFullAccess role to EC2 to allow CRUD on dynamodb tables</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2.4. Copy jar file to EC2 instance</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>java -jar aws-0.0.1-SNAPSHOT.jar</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2.6. Open app by using [your-own-ec2-instance-ip]:8080</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>First time open app could take a little bit of time to create table and insert data</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>[Add] button: To add new fortune</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Follow the link below (for windows user)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Check DynamoDB for item CRUD</t>
+    <phoneticPr fontId="4"/>
+  </si>
   <si>
     <r>
       <t xml:space="preserve">sudo yum </t>
@@ -75,90 +152,30 @@
       </rPr>
       <t>-amazon-corretto-headless</t>
     </r>
-  </si>
-  <si>
-    <t>Run as -&gt; Maven build … -&gt; Goals: package</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=qDTUYkaXAEc</t>
-  </si>
-  <si>
-    <t>https://intellipaat.com/community/43019/how-to-copy-files-from-local-machine-to-my-aws-instance</t>
-  </si>
-  <si>
-    <t>https://github.com/hn310/aws-challenge/tree/master/external-data/2_advanced_fortune_app</t>
-  </si>
-  <si>
-    <t>A. Manual</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>①．Build jar for "fortune of the day" spring project</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>・Option 1: Use the code in aws folder to customize on your own</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>・Option 2: Use aws-0.0.1-SNAPSHOT.jar if you want to deploy straight away without rebuilding the project</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>How to build jar in details</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>②．Create EC2</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2.1. Create EC2 instance with inbound allow port 8080</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2.2. Install java 11 on EC2 to run jar file</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2.3. Attach DynamoFullAccess role to EC2 to allow CRUD on dynamodb tables</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2.4. Copy jar file to EC2 instance</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2.5. Run jar file</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>java -jar aws-0.0.1-SNAPSHOT.jar</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2.6. Open app by using [your-own-ec2-instance-ip]:8080</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>First time open app could take a little bit of time to create table and insert data</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>[Add] button: To add new fortune</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>[Reset] button: To reset app state to initialized state (the state on above image)</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Follow the link below (for windows user)</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>Check DynamoDB for item CRUD</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>B. CloudFormation</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>①．Run advanced-fortune-ec2.yml to start EC2 Instance</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>②． Copy jar file to EC2 instance</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>[Reset] button: To reset app state to initialized state (the state on above image) (take some time to delete, create, insert data to DynamoDB)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>2.5. SSH to EC2, then run jar file</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>③．SSH to EC2, then run jar file</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -749,47 +766,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.69921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -797,13 +814,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -812,45 +829,45 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="D18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="E19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.45">
@@ -858,39 +875,74 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.45">
       <c r="E44" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="22.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C67" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E70" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E72" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -900,9 +952,10 @@
     <hyperlink ref="E19" r:id="rId2" xr:uid="{A547DE43-B144-445A-8821-B222A1B05EEC}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{AB507632-B5A3-4F63-850C-40161F331A67}"/>
     <hyperlink ref="D10" r:id="rId4" xr:uid="{5437FE45-2E26-43F3-AB4A-B2FA8EC49F1B}"/>
+    <hyperlink ref="E70" r:id="rId5" xr:uid="{10D9C0E9-E004-4C84-8E2E-396859E60CC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>